<commit_message>
final commit, everything is working
</commit_message>
<xml_diff>
--- a/data/locator_master.xlsx
+++ b/data/locator_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aerafkhan/PycharmProjects/sauceLabTestCases/pythonProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E90F055-868E-7048-80AF-A7956D335936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDFE0BA-05E5-F74B-A055-E0EDF16E1B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1840" windowWidth="28060" windowHeight="17200" xr2:uid="{32460D96-9436-2D41-A130-B8939B3EA704}"/>
+    <workbookView xWindow="1020" yWindow="1840" windowWidth="28060" windowHeight="17200" activeTab="1" xr2:uid="{32460D96-9436-2D41-A130-B8939B3EA704}"/>
   </bookViews>
   <sheets>
     <sheet name="android" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
   <si>
     <t>locator_name</t>
   </si>
@@ -277,6 +277,21 @@
   </si>
   <si>
     <t>com.saucelabs.mydemoapp.android:id/removeBt</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>checkout_page_checkout_title</t>
+  </si>
+  <si>
+    <t>com.saucelabs.mydemoapp.android:id/checkoutTitleTV</t>
+  </si>
+  <si>
+    <t>payment_page_checkout_title</t>
+  </si>
+  <si>
+    <t>com.saucelabs.mydemoapp.android:id/enterPaymentTitleTV</t>
   </si>
 </sst>
 </file>
@@ -648,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFDC768-66C8-C542-BD87-74B7EA78355D}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,144 +821,166 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>46</v>
       </c>
     </row>
@@ -954,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872EB03A-FC8C-594E-94CC-B39D5E4C2972}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="159" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,188 +1105,210 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>